<commit_message>
improved topic model using BERTopic and generated summaries
</commit_message>
<xml_diff>
--- a/tables/author_counts.xlsx
+++ b/tables/author_counts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,9 +457,6 @@
       <c r="G1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="n">
-        <v>14</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -485,9 +482,6 @@
       <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -513,9 +507,6 @@
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -541,9 +532,6 @@
       <c r="G4" t="n">
         <v>0</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -569,9 +557,6 @@
       <c r="G5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -597,9 +582,6 @@
       <c r="G6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -625,9 +607,6 @@
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -636,13 +615,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C8" t="n">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E8" t="n">
         <v>5</v>
@@ -653,9 +632,6 @@
       <c r="G8" t="n">
         <v>0</v>
       </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -664,16 +640,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D9" t="n">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E9" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F9" t="n">
         <v>6</v>
@@ -681,9 +657,6 @@
       <c r="G9" t="n">
         <v>0</v>
       </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -709,7 +682,29 @@
       <c r="G10" t="n">
         <v>4</v>
       </c>
-      <c r="H10" t="n">
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>(2025, 2035]</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>